<commit_message>
Data Driven Test Implementation in RestAssured
</commit_message>
<xml_diff>
--- a/src/test/resources/DDTest.xlsx
+++ b/src/test/resources/DDTest.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ltimindtree-my.sharepoint.com/personal/t_61096001_ltimindtree_com/Documents/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\61096001\eclipse-workspace\RestAssuredTraining\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_F25DC773A252ABDACC104836611850605BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BB35DEF-DD3F-46E8-AA1D-CE66C85EBBE2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1C0F76-B0DE-4A8D-96C9-8831C2400259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="RestAssured" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Testcases</t>
   </si>
@@ -66,19 +66,49 @@
   </si>
   <si>
     <t>payload</t>
+  </si>
+  <si>
+    <t>Learn Appium Automation with Java</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>isbn</t>
+  </si>
+  <si>
+    <t>aisle</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>RestAPI</t>
+  </si>
+  <si>
+    <t>Suriya Kumarr</t>
+  </si>
+  <si>
+    <t>fhhv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF17C6A3"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,8 +131,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -118,10 +149,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -389,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,12 +485,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF95CBE-0AE4-4309-A0BE-BC45A9623E42}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>637628</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>